<commit_message>
Updated Calibration data and edited Master for calibration of load cells
</commit_message>
<xml_diff>
--- a/Hardware/loadcell_calibration.xlsx
+++ b/Hardware/loadcell_calibration.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alexander\Documents\Documents\Cybathlon\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Anthony\Documents\College\Cybathlon\Code\cybathlon\Hardware\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BFC170D-A186-44DA-AE2E-1B18AA017284}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5563B1D-A52E-4C45-A35B-E9A620F98FA3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{BF80FCA8-9760-440F-ABE2-DDD5C9464224}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{BF80FCA8-9760-440F-ABE2-DDD5C9464224}"/>
   </bookViews>
   <sheets>
     <sheet name="LC1" sheetId="1" r:id="rId1"/>
@@ -56,12 +56,6 @@
     <t>Weight (N) (Actually weight + x)</t>
   </si>
   <si>
-    <t>Offset = -22702.69</t>
-  </si>
-  <si>
-    <t>y = x/7952.9 + 2.8546</t>
-  </si>
-  <si>
     <t>Offset</t>
   </si>
   <si>
@@ -69,6 +63,12 @@
   </si>
   <si>
     <t>1/Scale = 7952.9</t>
+  </si>
+  <si>
+    <t>Offset = 1.631336</t>
+  </si>
+  <si>
+    <t>y = x/7952.9 + 1.631336256</t>
   </si>
 </sst>
 </file>
@@ -4456,8 +4456,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B79A49BC-18AA-4E8C-8E5A-676B5BA32712}">
   <dimension ref="A1:H30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K32" sqref="K32"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N33" sqref="N33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4607,29 +4607,30 @@
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>0.15</v>
+        <v>2.53E-2</v>
       </c>
       <c r="B27">
         <f>A27*9.81</f>
-        <v>1.4715</v>
+        <v>0.248193</v>
       </c>
       <c r="H27" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="H28" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="H30" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -4638,7 +4639,7 @@
   <dimension ref="A1:I26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I25" sqref="I25"/>
+      <selection activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4796,31 +4797,31 @@
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="H25" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="I25" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>0.15</v>
+        <v>2.53E-2</v>
       </c>
       <c r="B26">
         <f>A26*9.81</f>
-        <v>1.4715</v>
+        <v>0.248193</v>
       </c>
       <c r="F26">
         <f>B26*8441.8</f>
-        <v>12422.108699999999</v>
+        <v>2095.1956673999998</v>
       </c>
       <c r="G26">
         <f>C2-F26</f>
-        <v>-78422.108699999997</v>
+        <v>-68095.195667399996</v>
       </c>
       <c r="H26">
         <f>G26*-1/8441.8</f>
-        <v>9.2897378165794038</v>
+        <v>8.0664308165794019</v>
       </c>
       <c r="I26">
         <v>8441.7999999999993</v>
@@ -4828,7 +4829,8 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -4837,7 +4839,7 @@
   <dimension ref="A1:I26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I25" sqref="I25"/>
+      <selection activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4995,31 +4997,31 @@
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="H25" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="I25" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>0.15</v>
+        <v>2.53E-2</v>
       </c>
       <c r="B26">
         <f>A26*9.81</f>
-        <v>1.4715</v>
+        <v>0.248193</v>
       </c>
       <c r="F26">
         <f>B26*7986</f>
-        <v>11751.398999999999</v>
+        <v>1982.0692979999999</v>
       </c>
       <c r="G26">
         <f>C2-F26</f>
-        <v>-52451.398999999998</v>
+        <v>-42682.069298000002</v>
       </c>
       <c r="H26">
         <f>G26*-1/7986</f>
-        <v>6.5679187327823687</v>
+        <v>5.3446117327823695</v>
       </c>
       <c r="I26">
         <v>7986</v>
@@ -5027,7 +5029,8 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -5035,8 +5038,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{387CCE21-7561-4678-B153-FE2B10E77F23}">
   <dimension ref="A1:I26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I25" sqref="I25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5194,31 +5197,31 @@
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="H25" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="I25" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>0.15</v>
+        <v>2.53E-2</v>
       </c>
       <c r="B26">
         <f>A26*9.81</f>
-        <v>1.4715</v>
+        <v>0.248193</v>
       </c>
       <c r="F26">
         <f>B26*8219.8</f>
-        <v>12095.4357</v>
+        <v>2040.0968213999997</v>
       </c>
       <c r="G26">
         <f>C2-F26</f>
-        <v>-49595.435700000002</v>
+        <v>-39540.096821400002</v>
       </c>
       <c r="H26">
         <f>G26*-1/8219.8</f>
-        <v>6.033654796953698</v>
+        <v>4.8103477969536979</v>
       </c>
       <c r="I26">
         <v>8219.7999999999993</v>
@@ -5226,6 +5229,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>